<commit_message>
Adding DB and Unix utils
</commit_message>
<xml_diff>
--- a/testScript/SuiteA/TestData.xlsx
+++ b/testScript/SuiteA/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11775" windowHeight="2220"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15705" windowHeight="6525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -394,7 +395,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,6 +403,7 @@
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>